<commit_message>
Add Selenium project Add more pick Tests refactor code
</commit_message>
<xml_diff>
--- a/ElementLogic.AMS.UI.Tests/ExcelDataAccess/UserCredentials/UserCredentials.xlsx
+++ b/ElementLogic.AMS.UI.Tests/ExcelDataAccess/UserCredentials/UserCredentials.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Key</t>
   </si>
@@ -36,7 +36,22 @@
     <t>adm</t>
   </si>
   <si>
-    <t>NormalUser</t>
+    <t>UserOne</t>
+  </si>
+  <si>
+    <t>UserTwo</t>
+  </si>
+  <si>
+    <t>UserThree</t>
+  </si>
+  <si>
+    <t>UserFour</t>
+  </si>
+  <si>
+    <t>UserFive</t>
+  </si>
+  <si>
+    <t>UserSix</t>
   </si>
 </sst>
 </file>
@@ -443,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -492,7 +507,61 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2040</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51041666666666696" footer="0.51041666666666696"/>
   <pageSetup paperSize="256" fitToWidth="0" fitToHeight="0" orientation="portrait" useFirstPageNumber="1"/>

</xml_diff>